<commit_message>
Added MLD code and modified excel sheet
</commit_message>
<xml_diff>
--- a/Generate_IxNetwork_Config-original.xlsx
+++ b/Generate_IxNetwork_Config-original.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\moharedd\Downloads\Cisco-cafy\latestcode\tgn_1812_latest\tgn_1812\Bulk-config\Mohan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF505539-47B9-45EB-9059-9EACC4AC6D78}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E06F3592-3052-43EE-9A21-1D442F3017DB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" firstSheet="7" activeTab="12" xr2:uid="{7E5D92D4-6857-044F-AF5A-65E71E62F3C3}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" firstSheet="11" activeTab="17" xr2:uid="{7E5D92D4-6857-044F-AF5A-65E71E62F3C3}"/>
   </bookViews>
   <sheets>
     <sheet name="Build_Information" sheetId="1" r:id="rId1"/>
@@ -29,12 +29,15 @@
     <sheet name="Network_Group" sheetId="4" r:id="rId14"/>
     <sheet name="IGMP_Host" sheetId="13" r:id="rId15"/>
     <sheet name="IGMP_Querier" sheetId="14" r:id="rId16"/>
-    <sheet name="DHCP_Ipv4" sheetId="21" r:id="rId17"/>
-    <sheet name="DHCP_Ipv6" sheetId="20" r:id="rId18"/>
-    <sheet name="DHCP_Serverv4" sheetId="22" r:id="rId19"/>
-    <sheet name="DHCP_Serverv6" sheetId="23" r:id="rId20"/>
-    <sheet name="Traffic" sheetId="9" r:id="rId21"/>
-    <sheet name="packet_editor" sheetId="17" r:id="rId22"/>
+    <sheet name="MLD_Host" sheetId="25" r:id="rId17"/>
+    <sheet name="MLD_Querier" sheetId="26" r:id="rId18"/>
+    <sheet name="DHCP_Ipv4" sheetId="21" r:id="rId19"/>
+    <sheet name="DHCP_Ipv6" sheetId="20" r:id="rId20"/>
+    <sheet name="DHCP_Serverv4" sheetId="22" r:id="rId21"/>
+    <sheet name="DHCP_Serverv6" sheetId="23" r:id="rId22"/>
+    <sheet name="LDP" sheetId="24" r:id="rId23"/>
+    <sheet name="Traffic" sheetId="9" r:id="rId24"/>
+    <sheet name="packet_editor" sheetId="17" r:id="rId25"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Devicegroup!$A$1:$I$38</definedName>
@@ -340,7 +343,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1478" uniqueCount="613">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1573" uniqueCount="639">
   <si>
     <t>yes</t>
   </si>
@@ -2179,6 +2182,84 @@
   </si>
   <si>
     <t>Enable 3-Way Handshake</t>
+  </si>
+  <si>
+    <t>Basic Hello Interval</t>
+  </si>
+  <si>
+    <t>Basic Hold Time</t>
+  </si>
+  <si>
+    <t>increment;10;1</t>
+  </si>
+  <si>
+    <t>increment;20;1</t>
+  </si>
+  <si>
+    <t>null</t>
+  </si>
+  <si>
+    <t>Enable BFD Registration</t>
+  </si>
+  <si>
+    <t>Enable Graceful Restart</t>
+  </si>
+  <si>
+    <t>Recovery Time</t>
+  </si>
+  <si>
+    <t>Reconnect Time</t>
+  </si>
+  <si>
+    <t>Keep Alive Interval</t>
+  </si>
+  <si>
+    <t>Keep Alive Hold Time</t>
+  </si>
+  <si>
+    <t>increment;190;1</t>
+  </si>
+  <si>
+    <t>increment;70;1</t>
+  </si>
+  <si>
+    <t>LDP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LDP Configuration </t>
+  </si>
+  <si>
+    <t>Router ID</t>
+  </si>
+  <si>
+    <t>194.100.0.1</t>
+  </si>
+  <si>
+    <t>increment;194.100.0.1;0.0.0.2</t>
+  </si>
+  <si>
+    <t>MLD Senders group Configuration</t>
+  </si>
+  <si>
+    <t>MLD Receivers Group Configuration</t>
+  </si>
+  <si>
+    <t>MLD_Host</t>
+  </si>
+  <si>
+    <t>MLD_Querier</t>
+  </si>
+  <si>
+    <t>ff04::1</t>
+  </si>
+  <si>
+    <t>ff03::1</t>
+  </si>
+  <si>
+    <t>aaaa::</t>
+  </si>
+  <si>
+    <t>aaaa:0:2::</t>
   </si>
 </sst>
 </file>
@@ -2581,35 +2662,6 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="24"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
       <numFmt numFmtId="30" formatCode="@"/>
       <fill>
         <patternFill>
@@ -2714,6 +2766,35 @@
         <scheme val="minor"/>
       </font>
     </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="24"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -2733,12 +2814,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{745DACF6-0076-3A46-9842-FCF5B835F442}" name="Table55" displayName="Table55" ref="B1:D15" totalsRowShown="0" headerRowDxfId="0" dataDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{745DACF6-0076-3A46-9842-FCF5B835F442}" name="Table55" displayName="Table55" ref="B1:D15" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
   <autoFilter ref="B1:D15" xr:uid="{51982F0C-E04B-7348-BA22-E3F6150ACF16}"/>
   <tableColumns count="3">
-    <tableColumn id="4" xr3:uid="{7A362E5A-1040-7149-8DBB-EC9D1844E05A}" name="Description" dataDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{D2425230-F6DB-144C-83EF-00D07B561F22}" name="Worksheet" dataDxfId="2"/>
-    <tableColumn id="1" xr3:uid="{E820C1AA-CB48-9E41-91AD-7A0AFBE94D0F}" name="Status" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{7A362E5A-1040-7149-8DBB-EC9D1844E05A}" name="Description" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{D2425230-F6DB-144C-83EF-00D07B561F22}" name="Worksheet" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{E820C1AA-CB48-9E41-91AD-7A0AFBE94D0F}" name="Status" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3044,10 +3125,10 @@
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
-  <dimension ref="A1:D22"/>
+  <dimension ref="A1:D25"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.1875" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
@@ -3342,27 +3423,69 @@
       <c r="A21" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B21" s="34" t="s">
+      <c r="B21" s="32" t="s">
+        <v>631</v>
+      </c>
+      <c r="C21" s="32" t="s">
+        <v>633</v>
+      </c>
+      <c r="D21" s="31" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="30.75" x14ac:dyDescent="0.9">
+      <c r="A22" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="B22" s="32" t="s">
+        <v>632</v>
+      </c>
+      <c r="C22" s="32" t="s">
+        <v>634</v>
+      </c>
+      <c r="D22" s="33" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="30.75" x14ac:dyDescent="0.9">
+      <c r="A23" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="B23" s="32" t="s">
+        <v>627</v>
+      </c>
+      <c r="C23" s="32" t="s">
+        <v>626</v>
+      </c>
+      <c r="D23" s="33" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="30.75" x14ac:dyDescent="0.9">
+      <c r="A24" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="B24" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="C21" s="34" t="s">
+      <c r="C24" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="D21" s="25" t="s">
+      <c r="D24" s="25" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="30.75" x14ac:dyDescent="0.9">
-      <c r="A22" s="35" t="s">
-        <v>0</v>
-      </c>
-      <c r="B22" s="36" t="s">
+    <row r="25" spans="1:4" ht="30.75" x14ac:dyDescent="0.9">
+      <c r="A25" s="35" t="s">
+        <v>0</v>
+      </c>
+      <c r="B25" s="36" t="s">
         <v>64</v>
       </c>
-      <c r="C22" s="36" t="s">
+      <c r="C25" s="36" t="s">
         <v>65</v>
       </c>
-      <c r="D22" s="33" t="s">
+      <c r="D25" s="33" t="s">
         <v>77</v>
       </c>
     </row>
@@ -4382,7 +4505,7 @@
   </sheetPr>
   <dimension ref="A1:T10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
+    <sheetView topLeftCell="P1" workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
@@ -5668,6 +5791,374 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A340CE4-7654-467F-825F-F684889D160A}">
+  <dimension ref="A1:L5"/>
+  <sheetViews>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.1875" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
+  <cols>
+    <col min="1" max="1" width="36.9375" customWidth="1"/>
+    <col min="2" max="2" width="23.75" customWidth="1"/>
+    <col min="3" max="3" width="37.6875" customWidth="1"/>
+    <col min="4" max="4" width="36.5625" customWidth="1"/>
+    <col min="5" max="11" width="34.8125" customWidth="1"/>
+    <col min="12" max="12" width="37.3125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" ht="30.75" x14ac:dyDescent="0.9">
+      <c r="A1" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>411</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>412</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>413</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>414</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>415</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>416</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>417</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>418</v>
+      </c>
+      <c r="J1" s="7" t="s">
+        <v>419</v>
+      </c>
+      <c r="K1" s="7" t="s">
+        <v>420</v>
+      </c>
+      <c r="L1" s="7" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="21" x14ac:dyDescent="0.65">
+      <c r="A2" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="B2" t="s">
+        <v>428</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
+        <v>635</v>
+      </c>
+      <c r="F2" t="s">
+        <v>542</v>
+      </c>
+      <c r="G2">
+        <v>10</v>
+      </c>
+      <c r="H2" t="s">
+        <v>439</v>
+      </c>
+      <c r="I2">
+        <v>1</v>
+      </c>
+      <c r="J2" t="s">
+        <v>637</v>
+      </c>
+      <c r="K2" t="s">
+        <v>542</v>
+      </c>
+      <c r="L2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="21" x14ac:dyDescent="0.65">
+      <c r="A3" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="B3" t="s">
+        <v>429</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+      <c r="E3" t="s">
+        <v>636</v>
+      </c>
+      <c r="F3" t="s">
+        <v>542</v>
+      </c>
+      <c r="G3">
+        <v>11</v>
+      </c>
+      <c r="H3" t="s">
+        <v>440</v>
+      </c>
+      <c r="I3">
+        <v>2</v>
+      </c>
+      <c r="J3" t="s">
+        <v>638</v>
+      </c>
+      <c r="K3" t="s">
+        <v>542</v>
+      </c>
+      <c r="L3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="21" x14ac:dyDescent="0.65">
+      <c r="A4" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="B4" t="s">
+        <v>430</v>
+      </c>
+      <c r="C4">
+        <v>3</v>
+      </c>
+      <c r="D4">
+        <v>3</v>
+      </c>
+      <c r="E4" t="s">
+        <v>635</v>
+      </c>
+      <c r="F4" t="s">
+        <v>542</v>
+      </c>
+      <c r="G4">
+        <v>12</v>
+      </c>
+      <c r="H4" t="s">
+        <v>439</v>
+      </c>
+      <c r="I4">
+        <v>3</v>
+      </c>
+      <c r="J4" t="s">
+        <v>637</v>
+      </c>
+      <c r="K4" t="s">
+        <v>542</v>
+      </c>
+      <c r="L4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="21" x14ac:dyDescent="0.65">
+      <c r="A5" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B5" t="s">
+        <v>429</v>
+      </c>
+      <c r="C5">
+        <v>4</v>
+      </c>
+      <c r="D5">
+        <v>4</v>
+      </c>
+      <c r="E5" t="s">
+        <v>636</v>
+      </c>
+      <c r="F5" t="s">
+        <v>542</v>
+      </c>
+      <c r="G5">
+        <v>13</v>
+      </c>
+      <c r="H5" t="s">
+        <v>440</v>
+      </c>
+      <c r="I5">
+        <v>4</v>
+      </c>
+      <c r="J5" t="s">
+        <v>638</v>
+      </c>
+      <c r="K5" t="s">
+        <v>542</v>
+      </c>
+      <c r="L5">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1CE1584-EA62-4567-9BC4-54EA9DB789C0}">
+  <dimension ref="A1:H5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.1875" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
+  <cols>
+    <col min="1" max="1" width="37.3125" customWidth="1"/>
+    <col min="2" max="2" width="18.5" customWidth="1"/>
+    <col min="3" max="3" width="28.9375" customWidth="1"/>
+    <col min="4" max="4" width="25.75" customWidth="1"/>
+    <col min="5" max="5" width="22.9375" customWidth="1"/>
+    <col min="6" max="6" width="21.6875" customWidth="1"/>
+    <col min="7" max="7" width="44.8125" customWidth="1"/>
+    <col min="8" max="8" width="38.8125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="30.75" x14ac:dyDescent="0.9">
+      <c r="A1" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>411</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>422</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>423</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>424</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>425</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>426</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="21" x14ac:dyDescent="0.65">
+      <c r="A2" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="B2" t="s">
+        <v>428</v>
+      </c>
+      <c r="C2">
+        <v>2</v>
+      </c>
+      <c r="D2">
+        <v>125</v>
+      </c>
+      <c r="E2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>2</v>
+      </c>
+      <c r="G2">
+        <v>10000</v>
+      </c>
+      <c r="H2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="21" x14ac:dyDescent="0.65">
+      <c r="A3" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="B3" t="s">
+        <v>429</v>
+      </c>
+      <c r="C3">
+        <v>3</v>
+      </c>
+      <c r="D3">
+        <v>126</v>
+      </c>
+      <c r="E3" t="b">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>3</v>
+      </c>
+      <c r="G3">
+        <v>11000</v>
+      </c>
+      <c r="H3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="21" x14ac:dyDescent="0.65">
+      <c r="A4" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="B4" t="s">
+        <v>430</v>
+      </c>
+      <c r="C4">
+        <v>4</v>
+      </c>
+      <c r="D4">
+        <v>127</v>
+      </c>
+      <c r="E4" t="b">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>4</v>
+      </c>
+      <c r="G4">
+        <v>12000</v>
+      </c>
+      <c r="H4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="21" x14ac:dyDescent="0.65">
+      <c r="A5" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="B5" t="s">
+        <v>428</v>
+      </c>
+      <c r="C5">
+        <v>5</v>
+      </c>
+      <c r="D5">
+        <v>128</v>
+      </c>
+      <c r="E5" t="b">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>5</v>
+      </c>
+      <c r="G5">
+        <v>13000</v>
+      </c>
+      <c r="H5">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FCC51B1-C11F-4C30-8C8B-A2E7A6EB3269}">
   <dimension ref="A1:I3"/>
   <sheetViews>
@@ -5769,264 +6260,6 @@
       </c>
       <c r="H3" t="s">
         <v>517</v>
-      </c>
-      <c r="I3" t="b">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{118B69DD-6F47-4236-9EAC-8456553696FA}">
-  <dimension ref="A1:L3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="A4:XFD4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.1875" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
-  <cols>
-    <col min="1" max="1" width="37.3125" customWidth="1"/>
-    <col min="2" max="2" width="40.25" customWidth="1"/>
-    <col min="3" max="3" width="42.0625" customWidth="1"/>
-    <col min="4" max="4" width="25.75" customWidth="1"/>
-    <col min="5" max="5" width="22.9375" customWidth="1"/>
-    <col min="6" max="6" width="28.25" customWidth="1"/>
-    <col min="7" max="8" width="44.8125" customWidth="1"/>
-    <col min="9" max="10" width="20.0625" customWidth="1"/>
-    <col min="11" max="11" width="27.75" customWidth="1"/>
-    <col min="12" max="12" width="44.8125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:12" ht="30.75" x14ac:dyDescent="0.9">
-      <c r="A1" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>520</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>509</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>510</v>
-      </c>
-      <c r="E1" s="7" t="s">
-        <v>511</v>
-      </c>
-      <c r="F1" s="7" t="s">
-        <v>512</v>
-      </c>
-      <c r="G1" s="7" t="s">
-        <v>521</v>
-      </c>
-      <c r="H1" s="7" t="s">
-        <v>522</v>
-      </c>
-      <c r="I1" s="7" t="s">
-        <v>524</v>
-      </c>
-      <c r="J1" s="7" t="s">
-        <v>525</v>
-      </c>
-      <c r="K1" s="7" t="s">
-        <v>526</v>
-      </c>
-      <c r="L1" s="7" t="s">
-        <v>523</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" ht="21" x14ac:dyDescent="0.65">
-      <c r="A2" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="B2" t="s">
-        <v>508</v>
-      </c>
-      <c r="C2" t="s">
-        <v>518</v>
-      </c>
-      <c r="D2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E2">
-        <v>0</v>
-      </c>
-      <c r="F2" t="b">
-        <v>0</v>
-      </c>
-      <c r="G2">
-        <v>1</v>
-      </c>
-      <c r="H2">
-        <v>1</v>
-      </c>
-      <c r="I2" t="s">
-        <v>529</v>
-      </c>
-      <c r="J2">
-        <v>10</v>
-      </c>
-      <c r="K2">
-        <v>1</v>
-      </c>
-      <c r="L2" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" ht="21" x14ac:dyDescent="0.65">
-      <c r="A3" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="B3" t="s">
-        <v>508</v>
-      </c>
-      <c r="C3" t="s">
-        <v>519</v>
-      </c>
-      <c r="D3" t="s">
-        <v>0</v>
-      </c>
-      <c r="E3">
-        <v>20</v>
-      </c>
-      <c r="F3" t="b">
-        <v>1</v>
-      </c>
-      <c r="G3">
-        <v>3</v>
-      </c>
-      <c r="H3">
-        <v>3</v>
-      </c>
-      <c r="I3" t="s">
-        <v>530</v>
-      </c>
-      <c r="J3">
-        <v>30</v>
-      </c>
-      <c r="K3">
-        <v>3</v>
-      </c>
-      <c r="L3" t="s">
-        <v>528</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{503026BC-0640-4254-BE5B-FF37C6FC99E2}">
-  <dimension ref="A1:J3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.1875" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
-  <cols>
-    <col min="1" max="1" width="37.3125" customWidth="1"/>
-    <col min="2" max="2" width="40.25" customWidth="1"/>
-    <col min="3" max="3" width="42.0625" customWidth="1"/>
-    <col min="4" max="4" width="21.3125" customWidth="1"/>
-    <col min="5" max="5" width="25.75" customWidth="1"/>
-    <col min="6" max="6" width="22.9375" customWidth="1"/>
-    <col min="7" max="7" width="28.25" customWidth="1"/>
-    <col min="8" max="8" width="27.1875" customWidth="1"/>
-    <col min="9" max="9" width="52.125" customWidth="1"/>
-    <col min="10" max="10" width="20.0625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10" ht="30.75" x14ac:dyDescent="0.9">
-      <c r="A1" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>531</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>532</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>536</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>533</v>
-      </c>
-      <c r="F1" s="7" t="s">
-        <v>535</v>
-      </c>
-      <c r="G1" s="7" t="s">
-        <v>537</v>
-      </c>
-      <c r="H1" s="7" t="s">
-        <v>512</v>
-      </c>
-      <c r="I1" s="7" t="s">
-        <v>538</v>
-      </c>
-      <c r="J1" s="7" t="s">
-        <v>539</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" ht="21" x14ac:dyDescent="0.65">
-      <c r="A2" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="B2" t="s">
-        <v>534</v>
-      </c>
-      <c r="C2" t="s">
-        <v>435</v>
-      </c>
-      <c r="D2">
-        <v>24</v>
-      </c>
-      <c r="E2">
-        <v>20</v>
-      </c>
-      <c r="F2">
-        <v>2</v>
-      </c>
-      <c r="G2">
-        <v>85400</v>
-      </c>
-      <c r="H2" t="b">
-        <v>0</v>
-      </c>
-      <c r="I2" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" ht="21" x14ac:dyDescent="0.65">
-      <c r="A3" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="B3" t="s">
-        <v>534</v>
-      </c>
-      <c r="C3" t="s">
-        <v>435</v>
-      </c>
-      <c r="D3">
-        <v>24</v>
-      </c>
-      <c r="E3">
-        <v>30</v>
-      </c>
-      <c r="F3">
-        <v>4</v>
-      </c>
-      <c r="G3">
-        <v>85000</v>
-      </c>
-      <c r="H3" t="b">
-        <v>0</v>
       </c>
       <c r="I3" t="b">
         <v>0</v>
@@ -6140,6 +6373,264 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{118B69DD-6F47-4236-9EAC-8456553696FA}">
+  <dimension ref="A1:L3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="A4:XFD4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.1875" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
+  <cols>
+    <col min="1" max="1" width="37.3125" customWidth="1"/>
+    <col min="2" max="2" width="40.25" customWidth="1"/>
+    <col min="3" max="3" width="42.0625" customWidth="1"/>
+    <col min="4" max="4" width="25.75" customWidth="1"/>
+    <col min="5" max="5" width="22.9375" customWidth="1"/>
+    <col min="6" max="6" width="28.25" customWidth="1"/>
+    <col min="7" max="8" width="44.8125" customWidth="1"/>
+    <col min="9" max="10" width="20.0625" customWidth="1"/>
+    <col min="11" max="11" width="27.75" customWidth="1"/>
+    <col min="12" max="12" width="44.8125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" ht="30.75" x14ac:dyDescent="0.9">
+      <c r="A1" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>520</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>509</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>510</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>511</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>512</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>521</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>522</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>524</v>
+      </c>
+      <c r="J1" s="7" t="s">
+        <v>525</v>
+      </c>
+      <c r="K1" s="7" t="s">
+        <v>526</v>
+      </c>
+      <c r="L1" s="7" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="21" x14ac:dyDescent="0.65">
+      <c r="A2" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="B2" t="s">
+        <v>508</v>
+      </c>
+      <c r="C2" t="s">
+        <v>518</v>
+      </c>
+      <c r="D2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="I2" t="s">
+        <v>529</v>
+      </c>
+      <c r="J2">
+        <v>10</v>
+      </c>
+      <c r="K2">
+        <v>1</v>
+      </c>
+      <c r="L2" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="21" x14ac:dyDescent="0.65">
+      <c r="A3" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="B3" t="s">
+        <v>508</v>
+      </c>
+      <c r="C3" t="s">
+        <v>519</v>
+      </c>
+      <c r="D3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>20</v>
+      </c>
+      <c r="F3" t="b">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <v>3</v>
+      </c>
+      <c r="H3">
+        <v>3</v>
+      </c>
+      <c r="I3" t="s">
+        <v>530</v>
+      </c>
+      <c r="J3">
+        <v>30</v>
+      </c>
+      <c r="K3">
+        <v>3</v>
+      </c>
+      <c r="L3" t="s">
+        <v>528</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{503026BC-0640-4254-BE5B-FF37C6FC99E2}">
+  <dimension ref="A1:J3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.1875" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
+  <cols>
+    <col min="1" max="1" width="37.3125" customWidth="1"/>
+    <col min="2" max="2" width="40.25" customWidth="1"/>
+    <col min="3" max="3" width="42.0625" customWidth="1"/>
+    <col min="4" max="4" width="21.3125" customWidth="1"/>
+    <col min="5" max="5" width="25.75" customWidth="1"/>
+    <col min="6" max="6" width="22.9375" customWidth="1"/>
+    <col min="7" max="7" width="28.25" customWidth="1"/>
+    <col min="8" max="8" width="27.1875" customWidth="1"/>
+    <col min="9" max="9" width="52.125" customWidth="1"/>
+    <col min="10" max="10" width="20.0625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="30.75" x14ac:dyDescent="0.9">
+      <c r="A1" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>531</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>532</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>536</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>533</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>535</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>537</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>512</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>538</v>
+      </c>
+      <c r="J1" s="7" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="21" x14ac:dyDescent="0.65">
+      <c r="A2" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="B2" t="s">
+        <v>534</v>
+      </c>
+      <c r="C2" t="s">
+        <v>435</v>
+      </c>
+      <c r="D2">
+        <v>24</v>
+      </c>
+      <c r="E2">
+        <v>20</v>
+      </c>
+      <c r="F2">
+        <v>2</v>
+      </c>
+      <c r="G2">
+        <v>85400</v>
+      </c>
+      <c r="H2" t="b">
+        <v>0</v>
+      </c>
+      <c r="I2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="21" x14ac:dyDescent="0.65">
+      <c r="A3" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="B3" t="s">
+        <v>534</v>
+      </c>
+      <c r="C3" t="s">
+        <v>435</v>
+      </c>
+      <c r="D3">
+        <v>24</v>
+      </c>
+      <c r="E3">
+        <v>30</v>
+      </c>
+      <c r="F3">
+        <v>4</v>
+      </c>
+      <c r="G3">
+        <v>85000</v>
+      </c>
+      <c r="H3" t="b">
+        <v>0</v>
+      </c>
+      <c r="I3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F803AC43-3B0B-40F2-9C09-A6F6972B791C}">
   <dimension ref="A1:L3"/>
   <sheetViews>
@@ -6282,7 +6773,158 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07579DF0-3E1D-4DC9-B8C6-91B7548A1D18}">
+  <dimension ref="A1:M3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.1875" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
+  <cols>
+    <col min="1" max="3" width="37.3125" customWidth="1"/>
+    <col min="4" max="4" width="40.25" customWidth="1"/>
+    <col min="5" max="5" width="42.0625" customWidth="1"/>
+    <col min="6" max="6" width="28.6875" customWidth="1"/>
+    <col min="7" max="7" width="25.75" customWidth="1"/>
+    <col min="8" max="8" width="40.125" customWidth="1"/>
+    <col min="9" max="9" width="28.25" customWidth="1"/>
+    <col min="10" max="10" width="27.1875" customWidth="1"/>
+    <col min="11" max="11" width="31.9375" customWidth="1"/>
+    <col min="12" max="12" width="42.125" customWidth="1"/>
+    <col min="13" max="13" width="28.375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" ht="30.75" x14ac:dyDescent="0.9">
+      <c r="A1" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>628</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>613</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>614</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>609</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>618</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>619</v>
+      </c>
+      <c r="J1" s="7" t="s">
+        <v>620</v>
+      </c>
+      <c r="K1" s="7" t="s">
+        <v>621</v>
+      </c>
+      <c r="L1" s="7" t="s">
+        <v>622</v>
+      </c>
+      <c r="M1" s="7" t="s">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="21" x14ac:dyDescent="0.65">
+      <c r="A2" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>461</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>629</v>
+      </c>
+      <c r="D2">
+        <v>10</v>
+      </c>
+      <c r="E2">
+        <v>20</v>
+      </c>
+      <c r="F2" t="s">
+        <v>617</v>
+      </c>
+      <c r="G2" t="s">
+        <v>407</v>
+      </c>
+      <c r="H2" t="b">
+        <v>0</v>
+      </c>
+      <c r="I2" t="b">
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <v>130000</v>
+      </c>
+      <c r="K2">
+        <v>130000</v>
+      </c>
+      <c r="L2">
+        <v>70</v>
+      </c>
+      <c r="M2">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="21" x14ac:dyDescent="0.65">
+      <c r="A3" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>630</v>
+      </c>
+      <c r="D3" t="s">
+        <v>615</v>
+      </c>
+      <c r="E3" t="s">
+        <v>616</v>
+      </c>
+      <c r="F3" t="s">
+        <v>373</v>
+      </c>
+      <c r="G3" t="s">
+        <v>408</v>
+      </c>
+      <c r="H3" t="b">
+        <v>1</v>
+      </c>
+      <c r="I3" t="b">
+        <v>1</v>
+      </c>
+      <c r="J3">
+        <v>130000</v>
+      </c>
+      <c r="K3">
+        <v>130000</v>
+      </c>
+      <c r="L3" t="s">
+        <v>625</v>
+      </c>
+      <c r="M3" t="s">
+        <v>624</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA67F99B-7122-014C-8188-F4470CB29FE9}">
   <sheetPr>
     <tabColor theme="9" tint="0.39997558519241921"/>
@@ -7690,7 +8332,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{305CDDC8-ED70-6A46-BC08-9987C1043545}">
   <sheetPr>
     <tabColor theme="9" tint="0.39997558519241921"/>

</xml_diff>